<commit_message>
2025.01.13_1 Backup from yesterday
</commit_message>
<xml_diff>
--- a/Analysis/Baseline_data_d1_exclusive.xlsx
+++ b/Analysis/Baseline_data_d1_exclusive.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gustavosplmoura/Library/Mobile Documents/com~apple~CloudDocs/Medicina/Biblioteca/Research/Data Science/Data Science/PROJECTS/DVEP/Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A024D2D-567F-554E-BF14-2D0F6DA5FB73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D1145D-AA3D-A34A-9F67-4AF1B8F00B74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20140" activeTab="2" xr2:uid="{704BFAC6-42D9-C841-B8C7-75AA64A2EC45}"/>
+    <workbookView xWindow="8320" yWindow="500" windowWidth="34560" windowHeight="20140" activeTab="2" xr2:uid="{704BFAC6-42D9-C841-B8C7-75AA64A2EC45}"/>
   </bookViews>
   <sheets>
     <sheet name="data_d1_exclusive" sheetId="2" r:id="rId1"/>
@@ -5282,7 +5282,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{248F0087-1006-CA47-A949-21AAD4381E95}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="A38" sqref="A38:D50"/>
     </sheetView>
   </sheetViews>
@@ -5772,8 +5772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64749C1A-EEE3-0F46-A684-D20DD1E92FA4}">
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="139" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51:H57"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="119" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -5783,7 +5783,7 @@
     <col min="3" max="3" width="6.59765625" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.3984375" style="1" customWidth="1"/>
     <col min="5" max="5" width="5.796875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11" style="1"/>
+    <col min="6" max="6" width="8.796875" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.3984375" style="2" customWidth="1"/>
     <col min="8" max="8" width="8.19921875" style="2" customWidth="1"/>
     <col min="9" max="9" width="8" style="2" customWidth="1"/>
@@ -6763,7 +6763,7 @@
     <mergeCell ref="E1:F1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="H2:I51 H53:I1048576 G52:H52">
+  <conditionalFormatting sqref="H2:I51 G52:H52 H53:I1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>

</xml_diff>